<commit_message>
Etykieta wersji aplkacji (dev czy prod)
</commit_message>
<xml_diff>
--- a/ExcelPln2/Input/PMI_VALID.xlsx
+++ b/ExcelPln2/Input/PMI_VALID.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="475" yWindow="421" windowWidth="19875" windowHeight="7648" activeTab="1"/>
+    <workbookView xWindow="475" yWindow="421" windowWidth="19875" windowHeight="7648"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="4" r:id="rId1"/>
@@ -8876,11 +8876,14 @@
   <sheetPr codeName="Arkusz1"/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -8916,7 +8919,7 @@
   <sheetPr codeName="Arkusz2"/>
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>

</xml_diff>